<commit_message>
[lab 2-5] Fix: refactor charts, Add: hints for user input
</commit_message>
<xml_diff>
--- a/app/templates/physics_2_5.xlsx
+++ b/app/templates/physics_2_5.xlsx
@@ -170,6 +170,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -177,17 +188,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -207,9 +207,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
@@ -219,6 +216,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -237,6 +243,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,15 +353,13 @@
           </spPr>
           <marker>
             <symbol val="circle"/>
-            <size val="5"/>
+            <size val="4"/>
             <spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="6350">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -367,6 +375,7 @@
             </spPr>
             <trendlineType val="poly"/>
             <order val="3"/>
+            <backward val="0.05000000000000001"/>
             <dispRSqr val="0"/>
             <dispEq val="0"/>
           </trendline>
@@ -407,25 +416,25 @@
                 <formatCode>General</formatCode>
                 <ptCount val="7"/>
                 <pt idx="0">
-                  <v>90.99999999999997</v>
+                  <v>100.1</v>
                 </pt>
                 <pt idx="1">
-                  <v>54.60000000000002</v>
+                  <v>54.59999999999998</v>
                 </pt>
                 <pt idx="2">
-                  <v>36.39999999999999</v>
+                  <v>45.50000000000001</v>
                 </pt>
                 <pt idx="3">
-                  <v>36.4</v>
+                  <v>27.30000000000001</v>
                 </pt>
                 <pt idx="4">
-                  <v>18.20000000000001</v>
+                  <v>27.29999999999999</v>
                 </pt>
                 <pt idx="5">
+                  <v>18.2</v>
+                </pt>
+                <pt idx="6">
                   <v>27.3</v>
-                </pt>
-                <pt idx="6">
-                  <v>18.2</v>
                 </pt>
               </numCache>
             </numRef>
@@ -454,15 +463,13 @@
           </spPr>
           <marker>
             <symbol val="circle"/>
-            <size val="5"/>
+            <size val="4"/>
             <spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="6350">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -517,25 +524,25 @@
                 <formatCode>General</formatCode>
                 <ptCount val="7"/>
                 <pt idx="0">
-                  <v>89.09999999999999</v>
+                  <v>93.2</v>
                 </pt>
                 <pt idx="1">
-                  <v>53.5</v>
+                  <v>55.9</v>
                 </pt>
                 <pt idx="2">
-                  <v>38.2</v>
+                  <v>39.9</v>
                 </pt>
                 <pt idx="3">
-                  <v>29.7</v>
+                  <v>31.1</v>
                 </pt>
                 <pt idx="4">
-                  <v>24.3</v>
+                  <v>25.4</v>
                 </pt>
                 <pt idx="5">
-                  <v>20.6</v>
+                  <v>21.5</v>
                 </pt>
                 <pt idx="6">
-                  <v>17.8</v>
+                  <v>18.6</v>
                 </pt>
               </numCache>
             </numRef>
@@ -820,15 +827,13 @@
           </spPr>
           <marker>
             <symbol val="circle"/>
-            <size val="5"/>
+            <size val="4"/>
             <spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+                <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -873,25 +878,25 @@
                 <formatCode>General</formatCode>
                 <ptCount val="8"/>
                 <pt idx="0">
-                  <v>3.094</v>
+                  <v>3.276</v>
                 </pt>
                 <pt idx="1">
-                  <v>2.184</v>
+                  <v>2.275</v>
                 </pt>
                 <pt idx="2">
-                  <v>1.638</v>
+                  <v>1.729</v>
                 </pt>
                 <pt idx="3">
                   <v>1.274</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.91</v>
+                  <v>1.001</v>
                 </pt>
                 <pt idx="5">
                   <v>0.728</v>
                 </pt>
                 <pt idx="6">
-                  <v>0.455</v>
+                  <v>0.546</v>
                 </pt>
                 <pt idx="7">
                   <v>0.273</v>
@@ -926,15 +931,13 @@
           </spPr>
           <marker>
             <symbol val="circle"/>
-            <size val="5"/>
+            <size val="4"/>
             <spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -979,28 +982,28 @@
                 <formatCode>General</formatCode>
                 <ptCount val="8"/>
                 <pt idx="0">
-                  <v>3.078</v>
+                  <v>3.217</v>
                 </pt>
                 <pt idx="1">
-                  <v>2.151</v>
+                  <v>2.249</v>
                 </pt>
                 <pt idx="2">
-                  <v>1.609</v>
+                  <v>1.682</v>
                 </pt>
                 <pt idx="3">
-                  <v>1.225</v>
+                  <v>1.28</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.926</v>
+                  <v>0.969</v>
                 </pt>
                 <pt idx="5">
-                  <v>0.6830000000000001</v>
+                  <v>0.714</v>
                 </pt>
                 <pt idx="6">
-                  <v>0.477</v>
+                  <v>0.498</v>
                 </pt>
                 <pt idx="7">
-                  <v>0.298</v>
+                  <v>0.312</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1252,7 +1255,7 @@
 <chartsheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1263,7 +1266,7 @@
 <chartsheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1581,7 +1584,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:A2"/>
@@ -1591,118 +1594,127 @@
   <cols>
     <col width="10.77734375" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="8.88671875" customWidth="1" min="4" max="5"/>
-    <col width="19.88671875" customWidth="1" min="6" max="6"/>
-    <col width="11.6640625" customWidth="1" min="7" max="7"/>
-    <col width="12.33203125" customWidth="1" min="8" max="8"/>
-    <col width="13.6640625" customWidth="1" min="9" max="9"/>
+    <col width="22.6640625" customWidth="1" min="6" max="6"/>
+    <col width="18.33203125" customWidth="1" min="7" max="7"/>
+    <col width="11.6640625" customWidth="1" min="8" max="8"/>
+    <col width="12.33203125" customWidth="1" min="9" max="9"/>
+    <col width="13.6640625" customWidth="1" min="10" max="10"/>
+    <col width="7.6640625" customWidth="1" min="11" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>Радіус r, см</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Струм I, мкА по променям</t>
         </is>
       </c>
-      <c r="C1" s="17" t="n"/>
-      <c r="D1" s="17" t="n"/>
-      <c r="E1" s="18" t="n"/>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="C1" s="19" t="n"/>
+      <c r="D1" s="19" t="n"/>
+      <c r="E1" s="20" t="n"/>
+      <c r="F1" s="21" t="inlineStr">
+        <is>
+          <t>Праворуч -&gt; краще нічого не змінювати, хіба що вам дуже хочеться;)</t>
+        </is>
+      </c>
+      <c r="G1" s="18" t="inlineStr">
         <is>
           <t>Точність окргуленя (знаків після коми)</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
-        <is>
-          <t>Зовнішній радіус rз, см</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>Внутрішний радіус rвн, см</t>
-        </is>
-      </c>
-      <c r="I1" s="16" t="inlineStr">
-        <is>
-          <t>Додактовий опір RД, кОм</t>
-        </is>
-      </c>
-      <c r="K1" s="8" t="inlineStr">
-        <is>
-          <t>Підписи графіків</t>
-        </is>
-      </c>
-      <c r="L1" s="9" t="n"/>
-      <c r="M1" s="9" t="n"/>
-      <c r="N1" s="10" t="n"/>
-      <c r="O1" s="14" t="inlineStr">
+      <c r="H1" s="18" t="inlineStr">
+        <is>
+          <t>Зовнішній радіус r з, см</t>
+        </is>
+      </c>
+      <c r="I1" s="18" t="inlineStr">
+        <is>
+          <t>Внутрішний радіус r вн, см</t>
+        </is>
+      </c>
+      <c r="J1" s="18" t="inlineStr">
+        <is>
+          <t>Додактовий опір Rд, кОм</t>
+        </is>
+      </c>
+      <c r="K1" s="10" t="inlineStr">
+        <is>
+          <t>Підписи осей графіків</t>
+        </is>
+      </c>
+      <c r="L1" s="11" t="n"/>
+      <c r="M1" s="11" t="n"/>
+      <c r="N1" s="12" t="n"/>
+      <c r="O1" s="16" t="inlineStr">
         <is>
           <t>U₀, В</t>
         </is>
       </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
-      <c r="A2" s="15" t="n"/>
-      <c r="B2" s="16" t="inlineStr">
+      <c r="A2" s="17" t="n"/>
+      <c r="B2" s="18" t="inlineStr">
         <is>
           <t>Промінь №1</t>
         </is>
       </c>
-      <c r="C2" s="16" t="inlineStr">
+      <c r="C2" s="18" t="inlineStr">
         <is>
           <t>Промінь №2</t>
         </is>
       </c>
-      <c r="D2" s="16" t="inlineStr">
+      <c r="D2" s="18" t="inlineStr">
         <is>
           <t>Промінь №3</t>
         </is>
       </c>
-      <c r="E2" s="16" t="inlineStr">
+      <c r="E2" s="18" t="inlineStr">
         <is>
           <t>Промінь №4</t>
         </is>
       </c>
-      <c r="F2" s="15" t="n"/>
-      <c r="G2" s="15" t="n"/>
-      <c r="H2" s="15" t="n"/>
-      <c r="I2" s="15" t="n"/>
-      <c r="K2" s="11" t="n"/>
-      <c r="L2" s="12" t="n"/>
-      <c r="M2" s="12" t="n"/>
-      <c r="N2" s="13" t="n"/>
-      <c r="O2" s="15" t="n"/>
+      <c r="F2" s="22" t="n"/>
+      <c r="G2" s="17" t="n"/>
+      <c r="H2" s="17" t="n"/>
+      <c r="I2" s="17" t="n"/>
+      <c r="J2" s="17" t="n"/>
+      <c r="K2" s="13" t="n"/>
+      <c r="L2" s="14" t="n"/>
+      <c r="M2" s="14" t="n"/>
+      <c r="N2" s="15" t="n"/>
+      <c r="O2" s="17" t="n"/>
     </row>
     <row r="3" ht="14.4" customHeight="1">
       <c r="A3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>45</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>45</v>
-      </c>
-      <c r="D3" s="6" t="n">
-        <v>45</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>45</v>
-      </c>
-      <c r="F3" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>49</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="F3" s="22" t="n"/>
+      <c r="G3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="J3" s="1" t="n">
         <v>91</v>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -1726,7 +1738,7 @@
         </is>
       </c>
       <c r="O3" s="1">
-        <f>Data!B3 * Data!I3 * 10^-3</f>
+        <f>Data!B3 * Data!J3 * 10^-3</f>
         <v/>
       </c>
     </row>
@@ -1735,16 +1747,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
@@ -1752,16 +1764,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1769,16 +1781,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -1786,16 +1798,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -1837,16 +1849,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -1854,28 +1866,46 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="8" t="inlineStr">
+        <is>
+          <t>↑                ↑                ↑                ↑</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="75.59999999999999" customHeight="1">
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>Однакові дані на променях виглядають трохи дивно…
+Якщо тобі це не подобається, то можеш зробити всі виміри вручну, може тоді боги усміхнуться тобі (ні)</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="K1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="F1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1904,60 +1934,60 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="16" t="inlineStr">
+      <c r="A1" s="18" t="inlineStr">
         <is>
           <t>Радіус r, см</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Струм I, мкА по променям</t>
         </is>
       </c>
-      <c r="C1" s="17" t="n"/>
-      <c r="D1" s="17" t="n"/>
-      <c r="E1" s="18" t="n"/>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="C1" s="19" t="n"/>
+      <c r="D1" s="19" t="n"/>
+      <c r="E1" s="20" t="n"/>
+      <c r="F1" s="18" t="inlineStr">
         <is>
           <t>Середній струм ⟨I₍ᵣ₎⟩, мкА</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>U, В</t>
         </is>
       </c>
-      <c r="H1" s="18" t="n"/>
+      <c r="H1" s="20" t="n"/>
     </row>
     <row r="2" ht="30" customHeight="1">
-      <c r="A2" s="15" t="n"/>
-      <c r="B2" s="16" t="inlineStr">
+      <c r="A2" s="17" t="n"/>
+      <c r="B2" s="18" t="inlineStr">
         <is>
           <t>Промінь №1</t>
         </is>
       </c>
-      <c r="C2" s="16" t="inlineStr">
+      <c r="C2" s="18" t="inlineStr">
         <is>
           <t>Промінь №2</t>
         </is>
       </c>
-      <c r="D2" s="16" t="inlineStr">
+      <c r="D2" s="18" t="inlineStr">
         <is>
           <t>Промінь №3</t>
         </is>
       </c>
-      <c r="E2" s="16" t="inlineStr">
+      <c r="E2" s="18" t="inlineStr">
         <is>
           <t>Промінь №4</t>
         </is>
       </c>
-      <c r="F2" s="15" t="n"/>
-      <c r="G2" s="16" t="inlineStr">
-        <is>
-          <t>Експерементальне U₍ᵣ₎=⟨I₍ᵣ₎⟩ · RД</t>
-        </is>
-      </c>
-      <c r="H2" s="16" t="inlineStr">
+      <c r="F2" s="17" t="n"/>
+      <c r="G2" s="18" t="inlineStr">
+        <is>
+          <t>Експерементальне U₍ᵣ₎=⟨I₍ᵣ₎⟩ · Rд</t>
+        </is>
+      </c>
+      <c r="H2" s="18" t="inlineStr">
         <is>
           <t>Теоретичне значення</t>
         </is>
@@ -1972,24 +2002,24 @@
         <v/>
       </c>
       <c r="C3" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1">
         <f>(B3+C3+D3+E3)/4</f>
         <v/>
       </c>
       <c r="G3" s="1">
-        <f>ROUND(F3 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F3 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H3" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A3) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A3) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -1998,27 +2028,27 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1">
         <f>(B4+C4+D4+E4)/4</f>
         <v/>
       </c>
       <c r="G4" s="1">
-        <f>ROUND(F4 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F4 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H4" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A4) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A4) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2027,27 +2057,27 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1">
         <f>(B5+C5+D5+E5)/4</f>
         <v/>
       </c>
       <c r="G5" s="1">
-        <f>ROUND(F5 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F5 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H5" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A5) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A5) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2072,11 +2102,11 @@
         <v/>
       </c>
       <c r="G6" s="1">
-        <f>ROUND(F6 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F6 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H6" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A6) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A6) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2085,27 +2115,27 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1">
         <f>(B7+C7+D7+E7)/4</f>
         <v/>
       </c>
       <c r="G7" s="1">
-        <f>ROUND(F7 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F7 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H7" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A7) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A7) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2130,11 +2160,11 @@
         <v/>
       </c>
       <c r="G8" s="1">
-        <f>ROUND(F8 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F8 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H8" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A8) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A8) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2143,27 +2173,27 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
         <f>(B9+C9+D9+E9)/4</f>
         <v/>
       </c>
       <c r="G9" s="1">
-        <f>ROUND(F9 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F9 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H9" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A9) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A9) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2188,11 +2218,11 @@
         <v/>
       </c>
       <c r="G10" s="1">
-        <f>ROUND(F10 * Data!$I$3 * 10^-3, Data!$F$3)</f>
+        <f>ROUND(F10 * Data!$J$3 * 10^-3, Data!$G$3)</f>
         <v/>
       </c>
       <c r="H10" s="1">
-        <f>ROUND(Data!$O$3 * LN(Data!$G$3/'Table 1'!A10) / LN(Data!$G$3/Data!$H$3), Data!$F$3)</f>
+        <f>ROUND(Data!$O$3 * LN(Data!$H$3/'Table 1'!A10) / LN(Data!$H$3/Data!$I$3), Data!$G$3)</f>
         <v/>
       </c>
     </row>
@@ -2264,22 +2294,22 @@
         <v/>
       </c>
       <c r="C2" s="1" t="n">
-        <v>54.60000000000002</v>
+        <v>54.59999999999998</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>36.39999999999999</v>
+        <v>45.50000000000001</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>36.4</v>
+        <v>27.30000000000001</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>18.20000000000001</v>
+        <v>27.29999999999999</v>
       </c>
       <c r="G2" s="1" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>27.3</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>18.2</v>
       </c>
     </row>
     <row r="3">
@@ -2289,31 +2319,31 @@
         </is>
       </c>
       <c r="B3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!B1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!B1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="C3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!C1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!C1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="D3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!D1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!D1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="E3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!E1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!E1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="F3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!F1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!F1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="G3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!G1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!G1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
       <c r="H3" s="1">
-        <f>ROUND(Data!$O$3 / 'Table 2'!H1 / LN(Data!$G$3/Data!$H$3) * 10^2, Data!$F$3-2)</f>
+        <f>ROUND(Data!$O$3 / 'Table 2'!H1 / LN(Data!$H$3/Data!$I$3) * 10^2, Data!$G$3-2)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
[lab 2-5] Remove: outdated hints
</commit_message>
<xml_diff>
--- a/app/templates/physics_2_5.xlsx
+++ b/app/templates/physics_2_5.xlsx
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -219,12 +219,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -416,16 +410,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="7"/>
                 <pt idx="0">
-                  <v>100.1</v>
+                  <v>109.2</v>
                 </pt>
                 <pt idx="1">
-                  <v>54.59999999999998</v>
+                  <v>54.6</v>
                 </pt>
                 <pt idx="2">
                   <v>45.50000000000001</v>
                 </pt>
                 <pt idx="3">
-                  <v>27.30000000000001</v>
+                  <v>36.40000000000001</v>
                 </pt>
                 <pt idx="4">
                   <v>27.29999999999999</v>
@@ -434,7 +428,7 @@
                   <v>18.2</v>
                 </pt>
                 <pt idx="6">
-                  <v>27.3</v>
+                  <v>18.20000000000001</v>
                 </pt>
               </numCache>
             </numRef>
@@ -524,25 +518,25 @@
                 <formatCode>General</formatCode>
                 <ptCount val="7"/>
                 <pt idx="0">
-                  <v>93.2</v>
+                  <v>99.2</v>
                 </pt>
                 <pt idx="1">
-                  <v>55.9</v>
+                  <v>59.5</v>
                 </pt>
                 <pt idx="2">
-                  <v>39.9</v>
+                  <v>42.5</v>
                 </pt>
                 <pt idx="3">
-                  <v>31.1</v>
+                  <v>33.1</v>
                 </pt>
                 <pt idx="4">
-                  <v>25.4</v>
+                  <v>27.1</v>
                 </pt>
                 <pt idx="5">
-                  <v>21.5</v>
+                  <v>22.9</v>
                 </pt>
                 <pt idx="6">
-                  <v>18.6</v>
+                  <v>19.8</v>
                 </pt>
               </numCache>
             </numRef>
@@ -604,7 +598,6 @@
               </a:p>
             </rich>
           </tx>
-          <layout/>
           <overlay val="0"/>
         </title>
         <numFmt formatCode="General" sourceLinked="1"/>
@@ -697,7 +690,6 @@
               </a:p>
             </rich>
           </tx>
-          <layout/>
           <overlay val="0"/>
         </title>
         <numFmt formatCode="General" sourceLinked="1"/>
@@ -755,7 +747,6 @@
         <idx val="3"/>
         <delete val="1"/>
       </legendEntry>
-      <layout/>
       <overlay val="0"/>
       <spPr>
         <a:noFill/>
@@ -878,16 +869,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="8"/>
                 <pt idx="0">
-                  <v>3.276</v>
+                  <v>3.458</v>
                 </pt>
                 <pt idx="1">
-                  <v>2.275</v>
+                  <v>2.366</v>
                 </pt>
                 <pt idx="2">
-                  <v>1.729</v>
+                  <v>1.82</v>
                 </pt>
                 <pt idx="3">
-                  <v>1.274</v>
+                  <v>1.365</v>
                 </pt>
                 <pt idx="4">
                   <v>1.001</v>
@@ -899,7 +890,7 @@
                   <v>0.546</v>
                 </pt>
                 <pt idx="7">
-                  <v>0.273</v>
+                  <v>0.364</v>
                 </pt>
               </numCache>
             </numRef>
@@ -982,28 +973,28 @@
                 <formatCode>General</formatCode>
                 <ptCount val="8"/>
                 <pt idx="0">
-                  <v>3.217</v>
+                  <v>3.427</v>
                 </pt>
                 <pt idx="1">
-                  <v>2.249</v>
+                  <v>2.396</v>
                 </pt>
                 <pt idx="2">
-                  <v>1.682</v>
+                  <v>1.792</v>
                 </pt>
                 <pt idx="3">
-                  <v>1.28</v>
+                  <v>1.364</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.969</v>
+                  <v>1.032</v>
                 </pt>
                 <pt idx="5">
-                  <v>0.714</v>
+                  <v>0.76</v>
                 </pt>
                 <pt idx="6">
-                  <v>0.498</v>
+                  <v>0.531</v>
                 </pt>
                 <pt idx="7">
-                  <v>0.312</v>
+                  <v>0.332</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1069,7 +1060,6 @@
               </a:p>
             </rich>
           </tx>
-          <layout/>
           <overlay val="0"/>
         </title>
         <numFmt formatCode="General" sourceLinked="1"/>
@@ -1162,7 +1152,6 @@
               </a:p>
             </rich>
           </tx>
-          <layout/>
           <overlay val="0"/>
         </title>
         <numFmt formatCode="General" sourceLinked="1"/>
@@ -1212,7 +1201,6 @@
     </plotArea>
     <legend>
       <legendPos val="r"/>
-      <layout/>
       <overlay val="0"/>
       <spPr>
         <a:noFill/>
@@ -1584,10 +1572,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1603,108 +1591,108 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="16" t="inlineStr">
         <is>
           <t>Радіус r, см</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Струм I, мкА по променям</t>
         </is>
       </c>
-      <c r="C1" s="19" t="n"/>
-      <c r="D1" s="19" t="n"/>
-      <c r="E1" s="20" t="n"/>
-      <c r="F1" s="21" t="inlineStr">
+      <c r="C1" s="17" t="n"/>
+      <c r="D1" s="17" t="n"/>
+      <c r="E1" s="18" t="n"/>
+      <c r="F1" s="19" t="inlineStr">
         <is>
           <t>Праворуч -&gt; краще нічого не змінювати, хіба що вам дуже хочеться;)</t>
         </is>
       </c>
-      <c r="G1" s="18" t="inlineStr">
+      <c r="G1" s="16" t="inlineStr">
         <is>
           <t>Точність окргуленя (знаків після коми)</t>
         </is>
       </c>
-      <c r="H1" s="18" t="inlineStr">
+      <c r="H1" s="16" t="inlineStr">
         <is>
           <t>Зовнішній радіус r з, см</t>
         </is>
       </c>
-      <c r="I1" s="18" t="inlineStr">
+      <c r="I1" s="16" t="inlineStr">
         <is>
           <t>Внутрішний радіус r вн, см</t>
         </is>
       </c>
-      <c r="J1" s="18" t="inlineStr">
+      <c r="J1" s="16" t="inlineStr">
         <is>
           <t>Додактовий опір Rд, кОм</t>
         </is>
       </c>
-      <c r="K1" s="10" t="inlineStr">
+      <c r="K1" s="8" t="inlineStr">
         <is>
           <t>Підписи осей графіків</t>
         </is>
       </c>
-      <c r="L1" s="11" t="n"/>
-      <c r="M1" s="11" t="n"/>
-      <c r="N1" s="12" t="n"/>
-      <c r="O1" s="16" t="inlineStr">
+      <c r="L1" s="9" t="n"/>
+      <c r="M1" s="9" t="n"/>
+      <c r="N1" s="10" t="n"/>
+      <c r="O1" s="14" t="inlineStr">
         <is>
           <t>U₀, В</t>
         </is>
       </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
-      <c r="A2" s="17" t="n"/>
-      <c r="B2" s="18" t="inlineStr">
+      <c r="A2" s="15" t="n"/>
+      <c r="B2" s="16" t="inlineStr">
         <is>
           <t>Промінь №1</t>
         </is>
       </c>
-      <c r="C2" s="18" t="inlineStr">
+      <c r="C2" s="16" t="inlineStr">
         <is>
           <t>Промінь №2</t>
         </is>
       </c>
-      <c r="D2" s="18" t="inlineStr">
+      <c r="D2" s="16" t="inlineStr">
         <is>
           <t>Промінь №3</t>
         </is>
       </c>
-      <c r="E2" s="18" t="inlineStr">
+      <c r="E2" s="16" t="inlineStr">
         <is>
           <t>Промінь №4</t>
         </is>
       </c>
-      <c r="F2" s="22" t="n"/>
-      <c r="G2" s="17" t="n"/>
-      <c r="H2" s="17" t="n"/>
-      <c r="I2" s="17" t="n"/>
-      <c r="J2" s="17" t="n"/>
-      <c r="K2" s="13" t="n"/>
-      <c r="L2" s="14" t="n"/>
-      <c r="M2" s="14" t="n"/>
-      <c r="N2" s="15" t="n"/>
-      <c r="O2" s="17" t="n"/>
+      <c r="F2" s="20" t="n"/>
+      <c r="G2" s="15" t="n"/>
+      <c r="H2" s="15" t="n"/>
+      <c r="I2" s="15" t="n"/>
+      <c r="J2" s="15" t="n"/>
+      <c r="K2" s="11" t="n"/>
+      <c r="L2" s="12" t="n"/>
+      <c r="M2" s="12" t="n"/>
+      <c r="N2" s="13" t="n"/>
+      <c r="O2" s="15" t="n"/>
     </row>
     <row r="3" ht="14.4" customHeight="1">
       <c r="A3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>49</v>
-      </c>
-      <c r="F3" s="22" t="n"/>
+        <v>46</v>
+      </c>
+      <c r="F3" s="20" t="n"/>
       <c r="G3" s="1" t="n">
         <v>3</v>
       </c>
@@ -1747,16 +1735,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -1764,16 +1752,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
@@ -1781,16 +1769,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -1798,16 +1786,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -1815,16 +1803,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -1852,13 +1840,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -1866,10 +1854,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>4</v>
@@ -1878,25 +1866,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>↑                ↑                ↑                ↑</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="75.59999999999999" customHeight="1">
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>Однакові дані на променях виглядають трохи дивно…
-Якщо тобі це не подобається, то можеш зробити всі виміри вручну, може тоді боги усміхнуться тобі (ні)</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
+  <mergeCells count="9">
     <mergeCell ref="K1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>
@@ -1934,60 +1905,60 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="inlineStr">
+      <c r="A1" s="16" t="inlineStr">
         <is>
           <t>Радіус r, см</t>
         </is>
       </c>
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Струм I, мкА по променям</t>
         </is>
       </c>
-      <c r="C1" s="19" t="n"/>
-      <c r="D1" s="19" t="n"/>
-      <c r="E1" s="20" t="n"/>
-      <c r="F1" s="18" t="inlineStr">
+      <c r="C1" s="17" t="n"/>
+      <c r="D1" s="17" t="n"/>
+      <c r="E1" s="18" t="n"/>
+      <c r="F1" s="16" t="inlineStr">
         <is>
           <t>Середній струм ⟨I₍ᵣ₎⟩, мкА</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>U, В</t>
         </is>
       </c>
-      <c r="H1" s="20" t="n"/>
+      <c r="H1" s="18" t="n"/>
     </row>
     <row r="2" ht="30" customHeight="1">
-      <c r="A2" s="17" t="n"/>
-      <c r="B2" s="18" t="inlineStr">
+      <c r="A2" s="15" t="n"/>
+      <c r="B2" s="16" t="inlineStr">
         <is>
           <t>Промінь №1</t>
         </is>
       </c>
-      <c r="C2" s="18" t="inlineStr">
+      <c r="C2" s="16" t="inlineStr">
         <is>
           <t>Промінь №2</t>
         </is>
       </c>
-      <c r="D2" s="18" t="inlineStr">
+      <c r="D2" s="16" t="inlineStr">
         <is>
           <t>Промінь №3</t>
         </is>
       </c>
-      <c r="E2" s="18" t="inlineStr">
+      <c r="E2" s="16" t="inlineStr">
         <is>
           <t>Промінь №4</t>
         </is>
       </c>
-      <c r="F2" s="17" t="n"/>
-      <c r="G2" s="18" t="inlineStr">
+      <c r="F2" s="15" t="n"/>
+      <c r="G2" s="16" t="inlineStr">
         <is>
           <t>Експерементальне U₍ᵣ₎=⟨I₍ᵣ₎⟩ · Rд</t>
         </is>
       </c>
-      <c r="H2" s="18" t="inlineStr">
+      <c r="H2" s="16" t="inlineStr">
         <is>
           <t>Теоретичне значення</t>
         </is>
@@ -2002,13 +1973,13 @@
         <v/>
       </c>
       <c r="C3" s="1" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F3" s="1">
         <f>(B3+C3+D3+E3)/4</f>
@@ -2028,16 +1999,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1">
         <f>(B4+C4+D4+E4)/4</f>
@@ -2057,16 +2028,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1">
         <f>(B5+C5+D5+E5)/4</f>
@@ -2086,16 +2057,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1">
         <f>(B6+C6+D6+E6)/4</f>
@@ -2202,16 +2173,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
         <f>(B10+C10+D10+E10)/4</f>
@@ -2294,13 +2265,13 @@
         <v/>
       </c>
       <c r="C2" s="1" t="n">
-        <v>54.59999999999998</v>
+        <v>54.6</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>45.50000000000001</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>27.30000000000001</v>
+        <v>36.40000000000001</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>27.29999999999999</v>
@@ -2309,7 +2280,7 @@
         <v>18.2</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>27.3</v>
+        <v>18.20000000000001</v>
       </c>
     </row>
     <row r="3">

</xml_diff>